<commit_message>
Restore code & spreadsheet from commit 401795f (no large artefacts)
</commit_message>
<xml_diff>
--- a/experiments/results/generalization_results.xlsx
+++ b/experiments/results/generalization_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programme\Nextcloud\00_Eigene_Dateien\Programmieren\dl_reference_models\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC2603-852C-4896-A42D-AFE179331385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8070F-CF66-4CD6-8126-9B69DA3D4AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <t>IMPALA</t>
   </si>
   <si>
-    <t>PPO 1.4, 3.1</t>
+    <t>PPO 1.2, 1.3, 1.4, 3.1</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +451,9 @@
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F2" s="4">
+        <v>1944000</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -468,6 +471,9 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="4">
+        <v>12816000</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -485,6 +491,9 @@
       <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="4">
+        <v>3824000</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -502,6 +511,9 @@
       <c r="E5" s="3">
         <v>89.7</v>
       </c>
+      <c r="F5" s="4">
+        <v>14360000</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -519,6 +531,9 @@
       <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F6" s="4">
+        <v>40090000</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -576,6 +591,9 @@
       <c r="E9" s="3">
         <v>90.1</v>
       </c>
+      <c r="F9" s="4">
+        <v>90598200</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -590,7 +608,9 @@
       <c r="D10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
@@ -599,10 +619,16 @@
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>8.6999999999999993</v>
+      </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>12.6</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">

</xml_diff>

<commit_message>
exp: update algorithm and mode in main.py; adjust checkpoint path and environment name
</commit_message>
<xml_diff>
--- a/experiments/results/generalization_results.xlsx
+++ b/experiments/results/generalization_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programme\Nextcloud\00_Eigene_Dateien\Programmieren\dl_reference_models\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8070F-CF66-4CD6-8126-9B69DA3D4AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13599460-4AC0-4938-BE02-98303B897771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>trained policy/ evaluation environment</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>PPO 1.2, 1.3, 1.4, 3.1</t>
+  </si>
+  <si>
+    <t>PPO 2.2, 3.1</t>
+  </si>
+  <si>
+    <t>because lowest successrate on 2.2</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +421,7 @@
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -455,7 +461,7 @@
         <v>1944000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -475,7 +481,7 @@
         <v>12816000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -495,7 +501,7 @@
         <v>3824000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -515,7 +521,7 @@
         <v>14360000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -535,7 +541,7 @@
         <v>40090000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -555,7 +561,7 @@
         <v>64861200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -575,7 +581,7 @@
         <v>56193900</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -595,7 +601,7 @@
         <v>90598200</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -615,23 +621,36 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="3">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3.1</v>
+      </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E11" s="3">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23.4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>14360000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
exp: finished experiments for generalization
</commit_message>
<xml_diff>
--- a/experiments/results/generalization_results.xlsx
+++ b/experiments/results/generalization_results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programme\Nextcloud\00_Eigene_Dateien\Programmieren\dl_reference_models\experiments\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nextcloud\00_Eigene_Dateien\Programmieren\dl_reference_models\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13599460-4AC0-4938-BE02-98303B897771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788F13A2-2C4F-42FA-8CB3-B242EFC72EA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>trained policy/ evaluation environment</t>
   </si>
@@ -66,9 +66,6 @@
     <t>env steps sampled</t>
   </si>
   <si>
-    <t>IMPALA</t>
-  </si>
-  <si>
     <t>PPO 1.2, 1.3, 1.4, 3.1</t>
   </si>
   <si>
@@ -76,6 +73,27 @@
   </si>
   <si>
     <t>because lowest successrate on 2.2</t>
+  </si>
+  <si>
+    <t>IMPALA 1.2, 1.3, 1.4, 3.1</t>
+  </si>
+  <si>
+    <t>IMPALA 2.2, 3.1</t>
+  </si>
+  <si>
+    <t>90,612,300</t>
+  </si>
+  <si>
+    <t>90,602,350</t>
+  </si>
+  <si>
+    <t>avg. Success rate</t>
+  </si>
+  <si>
+    <t>seed = 42</t>
+  </si>
+  <si>
+    <t>später mal mit 10 seeds und 100 samples machen?</t>
   </si>
 </sst>
 </file>
@@ -119,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -129,6 +147,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -409,19 +430,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,10 +459,13 @@
         <v>3.1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -457,11 +481,12 @@
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3"/>
+      <c r="G2" s="4">
         <v>1944000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -477,11 +502,12 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3"/>
+      <c r="G3" s="4">
         <v>12816000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -497,11 +523,12 @@
       <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3"/>
+      <c r="G4" s="4">
         <v>3824000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -517,11 +544,15 @@
       <c r="E5" s="3">
         <v>89.7</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
+        <f>AVERAGE(B5:E5)</f>
+        <v>34.299999999999997</v>
+      </c>
+      <c r="G5" s="4">
         <v>14360000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -537,11 +568,12 @@
       <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3"/>
+      <c r="G6" s="4">
         <v>40090000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -557,11 +589,12 @@
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3"/>
+      <c r="G7" s="4">
         <v>64861200</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -577,11 +610,12 @@
       <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3"/>
+      <c r="G8" s="4">
         <v>56193900</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -597,11 +631,15 @@
       <c r="E9" s="3">
         <v>90.1</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
+        <f t="shared" ref="F9:F14" si="0">AVERAGE(B9:E9)</f>
+        <v>47.125</v>
+      </c>
+      <c r="G9" s="4">
         <v>90598200</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -617,13 +655,17 @@
       <c r="E10" s="3">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3">
         <v>12</v>
@@ -637,24 +679,164 @@
       <c r="E11" s="3">
         <v>23.4</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>9.6749999999999989</v>
+      </c>
+      <c r="G11" s="4">
         <v>14360000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>88.5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>85.4</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>57.85</v>
+      </c>
+      <c r="G12" s="4">
+        <v>14360000</v>
+      </c>
+      <c r="H12" t="s">
         <v>15</v>
       </c>
-      <c r="G12" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="3">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>88.9</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>37.1</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>62.1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>88.1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>91.3</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>61.849999999999994</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: simplify dictionary initialization for actions and rewards in test_trained_model function
</commit_message>
<xml_diff>
--- a/experiments/results/generalization_results.xlsx
+++ b/experiments/results/generalization_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nextcloud\00_Eigene_Dateien\Programmieren\dl_reference_models\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788F13A2-2C4F-42FA-8CB3-B242EFC72EA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D7EF64-82C4-44C1-B162-07825381BD47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>PPO 2.2, 3.1</t>
   </si>
   <si>
-    <t>because lowest successrate on 2.2</t>
-  </si>
-  <si>
     <t>IMPALA 1.2, 1.3, 1.4, 3.1</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>später mal mit 10 seeds und 100 samples machen?</t>
+  </si>
+  <si>
+    <t>because lowest successrate on 2.2 decision to train additionally on it</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +459,7 @@
         <v>3.1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>12</v>
@@ -711,12 +711,12 @@
         <v>14360000</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3">
         <v>41</v>
@@ -735,12 +735,12 @@
         <v>37.1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3">
         <v>62.1</v>
@@ -759,15 +759,15 @@
         <v>61.849999999999994</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
         <v>21</v>
-      </c>
-      <c r="I16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -822,12 +822,12 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>